<commit_message>
Ajustes en nombres de recursos
Ajustes en nombres de recursos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion10/ESCALETA_FINAL_CN_10_10.xlsx
+++ b/fuentes/contenidos/grado10/guion10/ESCALETA_FINAL_CN_10_10.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado10\guion10\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -13,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$51</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -741,9 +746,6 @@
     <t>Competencias: estudio de las propiedades de los metales</t>
   </si>
   <si>
-    <t xml:space="preserve">Actividad que propone realizar un experimento para comparar las propiedades de algunos metales </t>
-  </si>
-  <si>
     <t>Resuelve el crucigrama sobre los elementos químicos</t>
   </si>
   <si>
@@ -821,10 +823,13 @@
     <t>Competencias: reconocimiento de espectros de emisión de metales</t>
   </si>
   <si>
-    <t>Actividad que propone una práctica de laboratorio para reconocer metales a través de sus espectros de emisión</t>
-  </si>
-  <si>
     <t>Recurso M102AB-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad que propone realizar una práctica de laboratorio comparar las propiedades de algunos metales </t>
+  </si>
+  <si>
+    <t>Actividad que propone una práctica de laboratorio para reconocer metales en sales a través de sus espectros de emisión</t>
   </si>
 </sst>
 </file>
@@ -1071,34 +1076,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1138,6 +1125,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1201,7 +1206,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1236,7 +1241,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1447,9 +1452,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U293"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K39" sqref="A39:XFD39"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1477,94 +1482,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="27" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="G1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="49" t="s">
+      <c r="K1" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="47" t="s">
+      <c r="L1" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="53" t="s">
+      <c r="M1" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="53"/>
-      <c r="O1" s="33" t="s">
+      <c r="N1" s="47"/>
+      <c r="O1" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="33" t="s">
+      <c r="P1" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="35" t="s">
+      <c r="Q1" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="39" t="s">
+      <c r="R1" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="35" t="s">
+      <c r="S1" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="37" t="s">
+      <c r="T1" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="35" t="s">
+      <c r="U1" s="50" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="27" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="46"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="48"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="42"/>
       <c r="M2" s="28" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="36"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="51"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="51"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -1591,7 +1596,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="32" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K3" s="24" t="s">
         <v>20</v>
@@ -1722,7 +1727,7 @@
       <c r="T6" s="12"/>
       <c r="U6" s="10"/>
     </row>
-    <row r="7" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>17</v>
       </c>
@@ -1749,7 +1754,7 @@
         <v>20</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>20</v>
@@ -1810,7 +1815,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>19</v>
@@ -1967,7 +1972,7 @@
         <v>20</v>
       </c>
       <c r="J11" s="30" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K11" s="7" t="s">
         <v>20</v>
@@ -2028,7 +2033,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="30" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K12" s="7" t="s">
         <v>19</v>
@@ -2237,7 +2242,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>17</v>
       </c>
@@ -2516,7 +2521,7 @@
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H23" s="21">
         <v>11</v>
@@ -2525,7 +2530,7 @@
         <v>19</v>
       </c>
       <c r="J23" s="30" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K23" s="7" t="s">
         <v>19</v>
@@ -3029,7 +3034,7 @@
         <v>149</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G33" s="16" t="s">
         <v>219</v>
@@ -3041,7 +3046,7 @@
         <v>20</v>
       </c>
       <c r="J33" s="17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K33" s="7" t="s">
         <v>19</v>
@@ -3100,7 +3105,7 @@
         <v>20</v>
       </c>
       <c r="J34" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K34" s="7" t="s">
         <v>20</v>
@@ -3279,7 +3284,7 @@
         <v>20</v>
       </c>
       <c r="J37" s="17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K37" s="7" t="s">
         <v>19</v>
@@ -3577,7 +3582,7 @@
       </c>
       <c r="F44" s="9"/>
       <c r="G44" s="16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H44" s="21">
         <v>25</v>
@@ -3586,7 +3591,7 @@
         <v>20</v>
       </c>
       <c r="J44" s="30" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K44" s="7" t="s">
         <v>19</v>
@@ -3610,7 +3615,7 @@
         <v>183</v>
       </c>
       <c r="T44" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U44" s="10" t="s">
         <v>184</v>
@@ -3634,7 +3639,7 @@
       </c>
       <c r="F45" s="9"/>
       <c r="G45" s="16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H45" s="21">
         <v>26</v>
@@ -3643,7 +3648,7 @@
         <v>20</v>
       </c>
       <c r="J45" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K45" s="7" t="s">
         <v>19</v>
@@ -3669,7 +3674,7 @@
         <v>183</v>
       </c>
       <c r="T45" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U45" s="10" t="s">
         <v>184</v>
@@ -3734,7 +3739,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="18" t="s">
         <v>17</v>
       </c>
@@ -3759,7 +3764,7 @@
         <v>20</v>
       </c>
       <c r="J47" s="30" t="s">
-        <v>240</v>
+        <v>266</v>
       </c>
       <c r="K47" s="7" t="s">
         <v>19</v>
@@ -3807,7 +3812,7 @@
       <c r="E48" s="13"/>
       <c r="F48" s="9"/>
       <c r="G48" s="16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H48" s="21">
         <v>29</v>
@@ -3816,7 +3821,7 @@
         <v>20</v>
       </c>
       <c r="J48" s="30" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="K48" s="7" t="s">
         <v>20</v>
@@ -3842,7 +3847,7 @@
         <v>188</v>
       </c>
       <c r="T48" s="12" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="U48" s="10" t="s">
         <v>190</v>
@@ -3859,7 +3864,7 @@
         <v>123</v>
       </c>
       <c r="D49" s="15" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E49" s="13"/>
       <c r="F49" s="9"/>
@@ -3873,7 +3878,7 @@
         <v>20</v>
       </c>
       <c r="J49" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K49" s="7" t="s">
         <v>20</v>
@@ -3904,12 +3909,12 @@
         <v>123</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E50" s="13"/>
       <c r="F50" s="9"/>
       <c r="G50" s="16" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H50" s="21">
         <v>31</v>
@@ -3918,7 +3923,7 @@
         <v>20</v>
       </c>
       <c r="J50" s="17" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K50" s="7" t="s">
         <v>20</v>
@@ -3944,7 +3949,7 @@
         <v>188</v>
       </c>
       <c r="T50" s="12" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="U50" s="10" t="s">
         <v>190</v>
@@ -3961,12 +3966,12 @@
         <v>123</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E51" s="13"/>
       <c r="F51" s="9"/>
       <c r="G51" s="16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H51" s="21">
         <v>32</v>
@@ -3975,7 +3980,7 @@
         <v>20</v>
       </c>
       <c r="J51" s="17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K51" s="7" t="s">
         <v>20</v>
@@ -4001,7 +4006,7 @@
         <v>188</v>
       </c>
       <c r="T51" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="U51" s="10" t="s">
         <v>190</v>
@@ -5014,6 +5019,12 @@
     <row r="293" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5028,12 +5039,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="O7" r:id="rId1"/>

</xml_diff>

<commit_message>
Cambio de nombre de recurso por espacio
Cambio de nombre de recurso por espacio
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion10/ESCALETA_FINAL_CN_10_10.xlsx
+++ b/fuentes/contenidos/grado10/guion10/ESCALETA_FINAL_CN_10_10.xlsx
@@ -802,9 +802,6 @@
     <t xml:space="preserve">Actividad para ampliar información sobre el átomo, sus componentes y los isótopos </t>
   </si>
   <si>
-    <t xml:space="preserve">La configuración electrónica de los elementos químicos </t>
-  </si>
-  <si>
     <t>Interactivo que permite conocer la distribución electrónica de algunos elementos y su relación con la ubicación en la tabla periódica</t>
   </si>
   <si>
@@ -830,6 +827,9 @@
   </si>
   <si>
     <t>Actividad que propone una práctica de laboratorio para reconocer metales en sales a través de sus espectros de emisión</t>
+  </si>
+  <si>
+    <t>La distribución electrónica</t>
   </si>
 </sst>
 </file>
@@ -1076,16 +1076,34 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1125,24 +1143,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1453,8 +1453,8 @@
   <dimension ref="A1:U293"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J53" sqref="J53"/>
+      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1482,94 +1482,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="27" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="45" t="s">
+      <c r="J1" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="43" t="s">
+      <c r="K1" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="41" t="s">
+      <c r="L1" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="47" t="s">
+      <c r="M1" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="47"/>
-      <c r="O1" s="35" t="s">
+      <c r="N1" s="53"/>
+      <c r="O1" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="50" t="s">
+      <c r="Q1" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="54" t="s">
+      <c r="R1" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="50" t="s">
+      <c r="S1" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="52" t="s">
+      <c r="T1" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="50" t="s">
+      <c r="U1" s="35" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="27" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="40"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="42"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="48"/>
       <c r="M2" s="28" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="51"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="36"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -2521,7 +2521,7 @@
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="16" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="H23" s="21">
         <v>11</v>
@@ -2530,7 +2530,7 @@
         <v>19</v>
       </c>
       <c r="J23" s="30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K23" s="7" t="s">
         <v>19</v>
@@ -3034,7 +3034,7 @@
         <v>149</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G33" s="16" t="s">
         <v>219</v>
@@ -3046,7 +3046,7 @@
         <v>20</v>
       </c>
       <c r="J33" s="17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K33" s="7" t="s">
         <v>19</v>
@@ -3105,7 +3105,7 @@
         <v>20</v>
       </c>
       <c r="J34" s="17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K34" s="7" t="s">
         <v>20</v>
@@ -3284,7 +3284,7 @@
         <v>20</v>
       </c>
       <c r="J37" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K37" s="7" t="s">
         <v>19</v>
@@ -3764,7 +3764,7 @@
         <v>20</v>
       </c>
       <c r="J47" s="30" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K47" s="7" t="s">
         <v>19</v>
@@ -3812,7 +3812,7 @@
       <c r="E48" s="13"/>
       <c r="F48" s="9"/>
       <c r="G48" s="16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H48" s="21">
         <v>29</v>
@@ -3821,7 +3821,7 @@
         <v>20</v>
       </c>
       <c r="J48" s="30" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K48" s="7" t="s">
         <v>20</v>
@@ -3847,7 +3847,7 @@
         <v>188</v>
       </c>
       <c r="T48" s="12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="U48" s="10" t="s">
         <v>190</v>
@@ -5019,12 +5019,6 @@
     <row r="293" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5039,6 +5033,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="O7" r:id="rId1"/>

</xml_diff>